<commit_message>
Actualizacion del proyecto web y correciones de doc.
se modifico el wbs, matris de rsponsabilidades y la herramienta de
riesgos ademas de restructurar la carpeta del proyecto web con un avance
del 90% satisfactorio
</commit_message>
<xml_diff>
--- a/Administracion-de-Proyectos/Planeacion-del-proyecto/Administracion-de-riesgos/TMv3-Herramienta para la Administración de Riesgos.xlsx
+++ b/Administracion-de-Proyectos/Planeacion-del-proyecto/Administracion-de-riesgos/TMv3-Herramienta para la Administración de Riesgos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2612" uniqueCount="497">
   <si>
     <t xml:space="preserve">El informe del resumen de los riesgos sintetiza el estado total de los riesgos en el proyecto.  </t>
   </si>
@@ -1830,19 +1830,55 @@
     <t>06/22/15</t>
   </si>
   <si>
-    <t>1.4.5</t>
-  </si>
-  <si>
-    <t>1.7.1</t>
-  </si>
-  <si>
-    <t>2.10.1</t>
-  </si>
-  <si>
     <t>1.2.3</t>
   </si>
   <si>
-    <t>1.4.4</t>
+    <t>1.3.5</t>
+  </si>
+  <si>
+    <t>1.2.2.12</t>
+  </si>
+  <si>
+    <t>1.2.2.11</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.1.6</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.5</t>
+  </si>
+  <si>
+    <t>1.1.8</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>1.1.9</t>
+  </si>
+  <si>
+    <t>1.2.2.6</t>
+  </si>
+  <si>
+    <t>1.2.1.5</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>1.2.2.11.1</t>
   </si>
 </sst>
 </file>
@@ -2432,7 +2468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3071,9 +3107,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3082,6 +3115,15 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3998,12 +4040,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="77451648"/>
-        <c:axId val="77453184"/>
-        <c:axId val="62900864"/>
+        <c:axId val="84821120"/>
+        <c:axId val="84822656"/>
+        <c:axId val="65854080"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="77451648"/>
+        <c:axId val="84821120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4048,7 +4090,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77453184"/>
+        <c:crossAx val="84822656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4058,7 +4100,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77453184"/>
+        <c:axId val="84822656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4103,13 +4145,13 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77451648"/>
+        <c:crossAx val="84821120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="62900864"/>
+        <c:axId val="65854080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4154,7 +4196,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77453184"/>
+        <c:crossAx val="84822656"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -6873,10 +6915,10 @@
       <c r="D15" s="197"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="238" t="s">
+      <c r="A16" s="237" t="s">
         <v>226</v>
       </c>
-      <c r="B16" s="239"/>
+      <c r="B16" s="238"/>
       <c r="C16" s="199"/>
       <c r="D16" s="199"/>
       <c r="E16" s="200"/>
@@ -6916,10 +6958,10 @@
       <c r="D21" s="197"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="238" t="s">
+      <c r="A22" s="237" t="s">
         <v>229</v>
       </c>
-      <c r="B22" s="239"/>
+      <c r="B22" s="238"/>
       <c r="C22" s="197"/>
       <c r="D22" s="197"/>
     </row>
@@ -6958,12 +7000,12 @@
       <c r="D27" s="197"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="238" t="s">
+      <c r="A28" s="237" t="s">
         <v>231</v>
       </c>
-      <c r="B28" s="240"/>
-      <c r="C28" s="240"/>
-      <c r="D28" s="239"/>
+      <c r="B28" s="239"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="238"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="196" t="s">
@@ -7879,8 +7921,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AB775"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F446" sqref="F446"/>
+    <sheetView tabSelected="1" topLeftCell="A553" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D571" sqref="D571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7953,8 +7995,8 @@
       <c r="B4" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="237">
-        <v>1.4</v>
+      <c r="C4" s="240" t="s">
+        <v>492</v>
       </c>
       <c r="D4" s="192"/>
       <c r="E4" s="21"/>
@@ -8455,8 +8497,8 @@
       <c r="B30" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="236" t="s">
-        <v>484</v>
+      <c r="C30" s="241" t="s">
+        <v>491</v>
       </c>
       <c r="D30" s="192"/>
       <c r="E30" s="21"/>
@@ -8986,8 +9028,8 @@
       <c r="B56" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C56" s="191">
-        <v>3</v>
+      <c r="C56" s="241" t="s">
+        <v>490</v>
       </c>
       <c r="D56" s="192"/>
       <c r="E56" s="21"/>
@@ -9455,8 +9497,8 @@
       <c r="B82" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C82" s="237">
-        <v>1.1000000000000001</v>
+      <c r="C82" s="240" t="s">
+        <v>489</v>
       </c>
       <c r="D82" s="192"/>
       <c r="E82" s="21"/>
@@ -9934,8 +9976,8 @@
       <c r="B108" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C108" s="236" t="s">
-        <v>480</v>
+      <c r="C108" s="241" t="s">
+        <v>488</v>
       </c>
       <c r="D108" s="192"/>
       <c r="E108" s="21"/>
@@ -10408,8 +10450,8 @@
       <c r="B133" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C133" s="191">
-        <v>3</v>
+      <c r="C133" s="236" t="s">
+        <v>487</v>
       </c>
       <c r="D133" s="192"/>
       <c r="E133" s="21"/>
@@ -10884,8 +10926,8 @@
       <c r="B159" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C159" s="237">
-        <v>2.11</v>
+      <c r="C159" s="240" t="s">
+        <v>487</v>
       </c>
       <c r="D159" s="192"/>
       <c r="E159" s="21"/>
@@ -11369,8 +11411,8 @@
       <c r="B185" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C185" s="237">
-        <v>1.6</v>
+      <c r="C185" s="240" t="s">
+        <v>486</v>
       </c>
       <c r="D185" s="192"/>
       <c r="E185" s="21"/>
@@ -11865,8 +11907,8 @@
       <c r="B211" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C211" s="236" t="s">
-        <v>480</v>
+      <c r="C211" s="241" t="s">
+        <v>485</v>
       </c>
       <c r="D211" s="192"/>
       <c r="E211" s="21"/>
@@ -12351,8 +12393,8 @@
       <c r="B237" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C237" s="237">
-        <v>1.4</v>
+      <c r="C237" s="240" t="s">
+        <v>484</v>
       </c>
       <c r="D237" s="192"/>
       <c r="E237" s="21"/>
@@ -12847,8 +12889,8 @@
       <c r="B263" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C263" s="191">
-        <v>2</v>
+      <c r="C263" s="241" t="s">
+        <v>483</v>
       </c>
       <c r="D263" s="192"/>
       <c r="E263" s="21"/>
@@ -13342,8 +13384,8 @@
       <c r="B289" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C289" s="191">
-        <v>2</v>
+      <c r="C289" s="241" t="s">
+        <v>482</v>
       </c>
       <c r="D289" s="192"/>
       <c r="E289" s="21"/>
@@ -13841,8 +13883,8 @@
       <c r="B315" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C315" s="191">
-        <v>4</v>
+      <c r="C315" s="236" t="s">
+        <v>481</v>
       </c>
       <c r="D315" s="192"/>
       <c r="E315" s="21"/>
@@ -14329,8 +14371,8 @@
       <c r="B341" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C341" s="191">
-        <v>3</v>
+      <c r="C341" s="236" t="s">
+        <v>493</v>
       </c>
       <c r="D341" s="192"/>
       <c r="E341" s="21"/>
@@ -14828,8 +14870,8 @@
       <c r="B367" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C367" s="237">
-        <v>1.1000000000000001</v>
+      <c r="C367" s="240" t="s">
+        <v>494</v>
       </c>
       <c r="D367" s="192"/>
       <c r="E367" s="21"/>
@@ -15323,8 +15365,8 @@
       <c r="B393" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C393" s="191">
-        <v>5</v>
+      <c r="C393" s="236" t="s">
+        <v>481</v>
       </c>
       <c r="D393" s="192"/>
       <c r="E393" s="21"/>
@@ -15818,8 +15860,8 @@
       <c r="B419" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C419" s="191">
-        <v>4</v>
+      <c r="C419" s="236" t="s">
+        <v>489</v>
       </c>
       <c r="D419" s="192"/>
       <c r="E419" s="21"/>
@@ -16303,8 +16345,8 @@
       <c r="B445" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C445" s="191">
-        <v>1</v>
+      <c r="C445" s="241" t="s">
+        <v>480</v>
       </c>
       <c r="D445" s="192"/>
       <c r="E445" s="21"/>
@@ -16789,7 +16831,7 @@
         <v>213</v>
       </c>
       <c r="C471" s="236" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="D471" s="192"/>
       <c r="E471" s="21"/>
@@ -17266,7 +17308,7 @@
         <v>213</v>
       </c>
       <c r="C496" s="236" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="D496" s="192"/>
       <c r="E496" s="21"/>
@@ -17742,8 +17784,8 @@
       <c r="B521" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C521" s="191">
-        <v>5</v>
+      <c r="C521" s="236" t="s">
+        <v>487</v>
       </c>
       <c r="D521" s="192"/>
       <c r="E521" s="21"/>
@@ -18209,8 +18251,8 @@
       <c r="B546" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C546" s="191">
-        <v>1</v>
+      <c r="C546" s="242">
+        <v>1.1000000000000001</v>
       </c>
       <c r="D546" s="192"/>
       <c r="E546" s="21"/>
@@ -18684,8 +18726,8 @@
       <c r="B572" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C572" s="191">
-        <v>1</v>
+      <c r="C572" s="242">
+        <v>1.1000000000000001</v>
       </c>
       <c r="D572" s="192"/>
       <c r="E572" s="21"/>
@@ -19151,8 +19193,8 @@
       <c r="B597" s="190" t="s">
         <v>213</v>
       </c>
-      <c r="C597" s="191">
-        <v>1</v>
+      <c r="C597" s="242">
+        <v>1.1000000000000001</v>
       </c>
       <c r="D597" s="192"/>
       <c r="E597" s="21"/>
@@ -19647,7 +19689,7 @@
         <v>213</v>
       </c>
       <c r="C623" s="236" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="D623" s="192"/>
       <c r="E623" s="21"/>
@@ -20127,7 +20169,7 @@
         <v>213</v>
       </c>
       <c r="C648" s="236" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="D648" s="192"/>
       <c r="E648" s="21"/>

</xml_diff>